<commit_message>
moved sound & video to storage
</commit_message>
<xml_diff>
--- a/documents/templates/Сводный бюджет_02_v23.xlsx
+++ b/documents/templates/Сводный бюджет_02_v23.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740" tabRatio="695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16240" tabRatio="695"/>
   </bookViews>
   <sheets>
-    <sheet name="Сводный" sheetId="1" r:id="rId1"/>
-    <sheet name="Продажи" sheetId="4" r:id="rId2"/>
-    <sheet name="Производство" sheetId="2" r:id="rId3"/>
-    <sheet name="Логистика" sheetId="3" r:id="rId4"/>
-    <sheet name="Прочее" sheetId="5" r:id="rId5"/>
+    <sheet name="Consolidated budget" sheetId="1" r:id="rId1"/>
+    <sheet name="Sales" sheetId="4" r:id="rId2"/>
+    <sheet name="Production" sheetId="2" r:id="rId3"/>
+    <sheet name="Logistics" sheetId="3" r:id="rId4"/>
+    <sheet name="Misc" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -795,13 +795,13 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -810,10 +810,10 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -823,14 +823,14 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -965,6 +965,15 @@
     <xf numFmtId="3" fontId="7" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="7" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -980,15 +989,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1369,65 +1369,65 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="8.625" style="1" customWidth="1"/>
-    <col min="14" max="18" width="9.625" style="1" customWidth="1"/>
+    <col min="2" max="13" width="8.6640625" style="1" customWidth="1"/>
+    <col min="14" max="18" width="9.6640625" style="1" customWidth="1"/>
     <col min="19" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="78" t="s">
+    <row r="1" spans="1:18" ht="15.75">
+      <c r="B1" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-    </row>
-    <row r="2" spans="1:18" s="28" customFormat="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="74" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+    </row>
+    <row r="2" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1"/>
+    <row r="3" spans="1:18" s="28" customFormat="1" ht="13">
+      <c r="B3" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="74" t="s">
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="77"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="86"/>
       <c r="R3" s="33" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="28" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1">
       <c r="B4" s="34">
         <v>1</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="28" customFormat="1" ht="13">
       <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
@@ -1502,56 +1502,56 @@
       <c r="Q5" s="43"/>
       <c r="R5" s="44"/>
     </row>
-    <row r="6" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3">
-        <f>Продажи!B6+Производство!B6+Логистика!B6+Прочее!B6</f>
+        <f>Sales!B6+Production!B6+Logistics!B6+Misc!B6</f>
         <v>585000</v>
       </c>
       <c r="C6" s="4">
-        <f>Продажи!C6+Производство!C6+Логистика!C6+Прочее!C6</f>
+        <f>Sales!C6+Production!C6+Logistics!C6+Misc!C6</f>
         <v>670000</v>
       </c>
       <c r="D6" s="4">
-        <f>Продажи!D6+Производство!D6+Логистика!D6+Прочее!D6</f>
+        <f>Sales!D6+Production!D6+Logistics!D6+Misc!D6</f>
         <v>628900</v>
       </c>
       <c r="E6" s="4">
-        <f>Продажи!E6+Производство!E6+Логистика!E6+Прочее!E6</f>
+        <f>Sales!E6+Production!E6+Logistics!E6+Misc!E6</f>
         <v>635732</v>
       </c>
       <c r="F6" s="4">
-        <f>Продажи!F6+Производство!F6+Логистика!F6+Прочее!F6</f>
+        <f>Sales!F6+Production!F6+Logistics!F6+Misc!F6</f>
         <v>574300</v>
       </c>
       <c r="G6" s="4">
-        <f>Продажи!G6+Производство!G6+Логистика!G6+Прочее!G6</f>
+        <f>Sales!G6+Production!G6+Logistics!G6+Misc!G6</f>
         <v>590543</v>
       </c>
       <c r="H6" s="4">
-        <f>Продажи!H6+Производство!H6+Логистика!H6+Прочее!H6</f>
+        <f>Sales!H6+Production!H6+Logistics!H6+Misc!H6</f>
         <v>600786</v>
       </c>
       <c r="I6" s="4">
-        <f>Продажи!I6+Производство!I6+Логистика!I6+Прочее!I6</f>
+        <f>Sales!I6+Production!I6+Logistics!I6+Misc!I6</f>
         <v>690434</v>
       </c>
       <c r="J6" s="4">
-        <f>Продажи!J6+Производство!J6+Логистика!J6+Прочее!J6</f>
+        <f>Sales!J6+Production!J6+Logistics!J6+Misc!J6</f>
         <v>765434</v>
       </c>
       <c r="K6" s="4">
-        <f>Продажи!K6+Производство!K6+Логистика!K6+Прочее!K6</f>
+        <f>Sales!K6+Production!K6+Logistics!K6+Misc!K6</f>
         <v>867532</v>
       </c>
       <c r="L6" s="4">
-        <f>Продажи!L6+Производство!L6+Логистика!L6+Прочее!L6</f>
+        <f>Sales!L6+Production!L6+Logistics!L6+Misc!L6</f>
         <v>900076</v>
       </c>
       <c r="M6" s="14">
-        <f>Продажи!M6+Производство!M6+Логистика!M6+Прочее!M6</f>
+        <f>Sales!M6+Production!M6+Logistics!M6+Misc!M6</f>
         <v>867534</v>
       </c>
       <c r="N6" s="3"/>
@@ -1560,56 +1560,56 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="15">
-        <f>Продажи!B7+Производство!B7+Логистика!B7+Прочее!B7</f>
+        <f>Sales!B7+Production!B7+Logistics!B7+Misc!B7</f>
         <v>1344</v>
       </c>
       <c r="C7" s="16">
-        <f>Продажи!C7+Производство!C7+Логистика!C7+Прочее!C7</f>
+        <f>Sales!C7+Production!C7+Logistics!C7+Misc!C7</f>
         <v>2144</v>
       </c>
       <c r="D7" s="16">
-        <f>Продажи!D7+Производство!D7+Логистика!D7+Прочее!D7</f>
+        <f>Sales!D7+Production!D7+Logistics!D7+Misc!D7</f>
         <v>5343</v>
       </c>
       <c r="E7" s="16">
-        <f>Продажи!E7+Производство!E7+Логистика!E7+Прочее!E7</f>
+        <f>Sales!E7+Production!E7+Logistics!E7+Misc!E7</f>
         <v>1298</v>
       </c>
       <c r="F7" s="16">
-        <f>Продажи!F7+Производство!F7+Логистика!F7+Прочее!F7</f>
+        <f>Sales!F7+Production!F7+Logistics!F7+Misc!F7</f>
         <v>1432</v>
       </c>
       <c r="G7" s="16">
-        <f>Продажи!G7+Производство!G7+Логистика!G7+Прочее!G7</f>
+        <f>Sales!G7+Production!G7+Logistics!G7+Misc!G7</f>
         <v>3786</v>
       </c>
       <c r="H7" s="16">
-        <f>Продажи!H7+Производство!H7+Логистика!H7+Прочее!H7</f>
+        <f>Sales!H7+Production!H7+Logistics!H7+Misc!H7</f>
         <v>2343</v>
       </c>
       <c r="I7" s="16">
-        <f>Продажи!I7+Производство!I7+Логистика!I7+Прочее!I7</f>
+        <f>Sales!I7+Production!I7+Logistics!I7+Misc!I7</f>
         <v>1243</v>
       </c>
       <c r="J7" s="16">
-        <f>Продажи!J7+Производство!J7+Логистика!J7+Прочее!J7</f>
+        <f>Sales!J7+Production!J7+Logistics!J7+Misc!J7</f>
         <v>2333</v>
       </c>
       <c r="K7" s="16">
-        <f>Продажи!K7+Производство!K7+Логистика!K7+Прочее!K7</f>
+        <f>Sales!K7+Production!K7+Logistics!K7+Misc!K7</f>
         <v>3005</v>
       </c>
       <c r="L7" s="16">
-        <f>Продажи!L7+Производство!L7+Логистика!L7+Прочее!L7</f>
+        <f>Sales!L7+Production!L7+Logistics!L7+Misc!L7</f>
         <v>2556</v>
       </c>
       <c r="M7" s="17">
-        <f>Продажи!M7+Производство!M7+Логистика!M7+Прочее!M7</f>
+        <f>Sales!M7+Production!M7+Logistics!M7+Misc!M7</f>
         <v>2765</v>
       </c>
       <c r="N7" s="15"/>
@@ -1618,7 +1618,7 @@
       <c r="Q7" s="18"/>
       <c r="R7" s="19"/>
     </row>
-    <row r="8" spans="1:18" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="28" customFormat="1" ht="15.75" thickBot="1">
       <c r="A8" s="20" t="s">
         <v>3</v>
       </c>
@@ -1676,7 +1676,7 @@
       <c r="Q8" s="26"/>
       <c r="R8" s="27"/>
     </row>
-    <row r="9" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="28" customFormat="1" ht="13">
       <c r="A9" s="39" t="s">
         <v>4</v>
       </c>
@@ -1698,56 +1698,56 @@
       <c r="Q9" s="50"/>
       <c r="R9" s="51"/>
     </row>
-    <row r="10" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="3">
-        <f>Продажи!B10+Производство!B10+Логистика!B10+Прочее!B10</f>
+        <f>Sales!B10+Production!B10+Logistics!B10+Misc!B10</f>
         <v>250000</v>
       </c>
       <c r="C10" s="4">
-        <f>Продажи!C10+Производство!C10+Логистика!C10+Прочее!C10</f>
+        <f>Sales!C10+Production!C10+Logistics!C10+Misc!C10</f>
         <v>191250</v>
       </c>
       <c r="D10" s="4">
-        <f>Продажи!D10+Производство!D10+Логистика!D10+Прочее!D10</f>
+        <f>Sales!D10+Production!D10+Logistics!D10+Misc!D10</f>
         <v>150830.83333333334</v>
       </c>
       <c r="E10" s="4">
-        <f>Продажи!E10+Производство!E10+Логистика!E10+Прочее!E10</f>
+        <f>Sales!E10+Production!E10+Logistics!E10+Misc!E10</f>
         <v>185891.66666666669</v>
       </c>
       <c r="F10" s="4">
-        <f>Продажи!F10+Производство!F10+Логистика!F10+Прочее!F10</f>
+        <f>Sales!F10+Production!F10+Logistics!F10+Misc!F10</f>
         <v>100441.66666666667</v>
       </c>
       <c r="G10" s="4">
-        <f>Продажи!G10+Производство!G10+Логистика!G10+Прочее!G10</f>
+        <f>Sales!G10+Production!G10+Logistics!G10+Misc!G10</f>
         <v>139916.66666666669</v>
       </c>
       <c r="H10" s="4">
-        <f>Продажи!H10+Производство!H10+Логистика!H10+Прочее!H10</f>
+        <f>Sales!H10+Production!H10+Logistics!H10+Misc!H10</f>
         <v>187250</v>
       </c>
       <c r="I10" s="4">
-        <f>Продажи!I10+Производство!I10+Логистика!I10+Прочее!I10</f>
+        <f>Sales!I10+Production!I10+Logistics!I10+Misc!I10</f>
         <v>292139.16666666669</v>
       </c>
       <c r="J10" s="4">
-        <f>Продажи!J10+Производство!J10+Логистика!J10+Прочее!J10</f>
+        <f>Sales!J10+Production!J10+Logistics!J10+Misc!J10</f>
         <v>192239.16666666669</v>
       </c>
       <c r="K10" s="4">
-        <f>Продажи!K10+Производство!K10+Логистика!K10+Прочее!K10</f>
+        <f>Sales!K10+Production!K10+Logistics!K10+Misc!K10</f>
         <v>149120.83333333334</v>
       </c>
       <c r="L10" s="4">
-        <f>Продажи!L10+Производство!L10+Логистика!L10+Прочее!L10</f>
+        <f>Sales!L10+Production!L10+Logistics!L10+Misc!L10</f>
         <v>155583.33333333334</v>
       </c>
       <c r="M10" s="5">
-        <f>Продажи!M10+Производство!M10+Логистика!M10+Прочее!M10</f>
+        <f>Sales!M10+Production!M10+Logistics!M10+Misc!M10</f>
         <v>102791.66666666667</v>
       </c>
       <c r="N10" s="6"/>
@@ -1756,56 +1756,56 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="3">
-        <f>Продажи!B11+Производство!B11+Логистика!B11+Прочее!B11</f>
+        <f>Sales!B11+Production!B11+Logistics!B11+Misc!B11</f>
         <v>0</v>
       </c>
       <c r="C11" s="4">
-        <f>Продажи!C11+Производство!C11+Логистика!C11+Прочее!C11</f>
+        <f>Sales!C11+Production!C11+Logistics!C11+Misc!C11</f>
         <v>0</v>
       </c>
       <c r="D11" s="4">
-        <f>Продажи!D11+Производство!D11+Логистика!D11+Прочее!D11</f>
+        <f>Sales!D11+Production!D11+Logistics!D11+Misc!D11</f>
         <v>0</v>
       </c>
       <c r="E11" s="4">
-        <f>Продажи!E11+Производство!E11+Логистика!E11+Прочее!E11</f>
+        <f>Sales!E11+Production!E11+Logistics!E11+Misc!E11</f>
         <v>0</v>
       </c>
       <c r="F11" s="4">
-        <f>Продажи!F11+Производство!F11+Логистика!F11+Прочее!F11</f>
+        <f>Sales!F11+Production!F11+Logistics!F11+Misc!F11</f>
         <v>0</v>
       </c>
       <c r="G11" s="4">
-        <f>Продажи!G11+Производство!G11+Логистика!G11+Прочее!G11</f>
+        <f>Sales!G11+Production!G11+Logistics!G11+Misc!G11</f>
         <v>0</v>
       </c>
       <c r="H11" s="4">
-        <f>Продажи!H11+Производство!H11+Логистика!H11+Прочее!H11</f>
+        <f>Sales!H11+Production!H11+Logistics!H11+Misc!H11</f>
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <f>Продажи!I11+Производство!I11+Логистика!I11+Прочее!I11</f>
+        <f>Sales!I11+Production!I11+Logistics!I11+Misc!I11</f>
         <v>0</v>
       </c>
       <c r="J11" s="4">
-        <f>Продажи!J11+Производство!J11+Логистика!J11+Прочее!J11</f>
+        <f>Sales!J11+Production!J11+Logistics!J11+Misc!J11</f>
         <v>0</v>
       </c>
       <c r="K11" s="4">
-        <f>Продажи!K11+Производство!K11+Логистика!K11+Прочее!K11</f>
+        <f>Sales!K11+Production!K11+Logistics!K11+Misc!K11</f>
         <v>0</v>
       </c>
       <c r="L11" s="4">
-        <f>Продажи!L11+Производство!L11+Логистика!L11+Прочее!L11</f>
+        <f>Sales!L11+Production!L11+Logistics!L11+Misc!L11</f>
         <v>0</v>
       </c>
       <c r="M11" s="5">
-        <f>Продажи!M11+Производство!M11+Логистика!M11+Прочее!M11</f>
+        <f>Sales!M11+Production!M11+Logistics!M11+Misc!M11</f>
         <v>0</v>
       </c>
       <c r="N11" s="6"/>
@@ -1814,56 +1814,56 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3">
-        <f>Продажи!B12+Производство!B12+Логистика!B12+Прочее!B12</f>
+        <f>Sales!B12+Production!B12+Logistics!B12+Misc!B12</f>
         <v>22500</v>
       </c>
       <c r="C12" s="4">
-        <f>Продажи!C12+Производство!C12+Логистика!C12+Прочее!C12</f>
+        <f>Sales!C12+Production!C12+Logistics!C12+Misc!C12</f>
         <v>22321</v>
       </c>
       <c r="D12" s="4">
-        <f>Продажи!D12+Производство!D12+Логистика!D12+Прочее!D12</f>
+        <f>Sales!D12+Production!D12+Logistics!D12+Misc!D12</f>
         <v>19670</v>
       </c>
       <c r="E12" s="4">
-        <f>Продажи!E12+Производство!E12+Логистика!E12+Прочее!E12</f>
+        <f>Sales!E12+Production!E12+Logistics!E12+Misc!E12</f>
         <v>18709</v>
       </c>
       <c r="F12" s="4">
-        <f>Продажи!F12+Производство!F12+Логистика!F12+Прочее!F12</f>
+        <f>Sales!F12+Production!F12+Logistics!F12+Misc!F12</f>
         <v>24387</v>
       </c>
       <c r="G12" s="4">
-        <f>Продажи!G12+Производство!G12+Логистика!G12+Прочее!G12</f>
+        <f>Sales!G12+Production!G12+Logistics!G12+Misc!G12</f>
         <v>15087</v>
       </c>
       <c r="H12" s="4">
-        <f>Продажи!H12+Производство!H12+Логистика!H12+Прочее!H12</f>
+        <f>Sales!H12+Production!H12+Logistics!H12+Misc!H12</f>
         <v>23001</v>
       </c>
       <c r="I12" s="4">
-        <f>Продажи!I12+Производство!I12+Логистика!I12+Прочее!I12</f>
+        <f>Sales!I12+Production!I12+Logistics!I12+Misc!I12</f>
         <v>15003</v>
       </c>
       <c r="J12" s="4">
-        <f>Продажи!J12+Производство!J12+Логистика!J12+Прочее!J12</f>
+        <f>Sales!J12+Production!J12+Logistics!J12+Misc!J12</f>
         <v>16089</v>
       </c>
       <c r="K12" s="4">
-        <f>Продажи!K12+Производство!K12+Логистика!K12+Прочее!K12</f>
+        <f>Sales!K12+Production!K12+Logistics!K12+Misc!K12</f>
         <v>19800</v>
       </c>
       <c r="L12" s="4">
-        <f>Продажи!L12+Производство!L12+Логистика!L12+Прочее!L12</f>
+        <f>Sales!L12+Production!L12+Logistics!L12+Misc!L12</f>
         <v>23670</v>
       </c>
       <c r="M12" s="5">
-        <f>Продажи!M12+Производство!M12+Логистика!M12+Прочее!M12</f>
+        <f>Sales!M12+Production!M12+Logistics!M12+Misc!M12</f>
         <v>24100</v>
       </c>
       <c r="N12" s="6"/>
@@ -1872,56 +1872,56 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3">
-        <f>Продажи!B13+Производство!B13+Логистика!B13+Прочее!B13</f>
+        <f>Sales!B13+Production!B13+Logistics!B13+Misc!B13</f>
         <v>125640</v>
       </c>
       <c r="C13" s="4">
-        <f>Продажи!C13+Производство!C13+Логистика!C13+Прочее!C13</f>
+        <f>Sales!C13+Production!C13+Logistics!C13+Misc!C13</f>
         <v>119220</v>
       </c>
       <c r="D13" s="4">
-        <f>Продажи!D13+Производство!D13+Логистика!D13+Прочее!D13</f>
+        <f>Sales!D13+Production!D13+Logistics!D13+Misc!D13</f>
         <v>115585</v>
       </c>
       <c r="E13" s="4">
-        <f>Продажи!E13+Производство!E13+Логистика!E13+Прочее!E13</f>
+        <f>Sales!E13+Production!E13+Logistics!E13+Misc!E13</f>
         <v>121830</v>
       </c>
       <c r="F13" s="4">
-        <f>Продажи!F13+Производство!F13+Логистика!F13+Прочее!F13</f>
+        <f>Sales!F13+Production!F13+Logistics!F13+Misc!F13</f>
         <v>107443</v>
       </c>
       <c r="G13" s="4">
-        <f>Продажи!G13+Производство!G13+Логистика!G13+Прочее!G13</f>
+        <f>Sales!G13+Production!G13+Logistics!G13+Misc!G13</f>
         <v>114646</v>
       </c>
       <c r="H13" s="4">
-        <f>Продажи!H13+Производство!H13+Логистика!H13+Прочее!H13</f>
+        <f>Sales!H13+Production!H13+Logistics!H13+Misc!H13</f>
         <v>124900</v>
       </c>
       <c r="I13" s="4">
-        <f>Продажи!I13+Производство!I13+Логистика!I13+Прочее!I13</f>
+        <f>Sales!I13+Production!I13+Logistics!I13+Misc!I13</f>
         <v>121379</v>
       </c>
       <c r="J13" s="4">
-        <f>Продажи!J13+Производство!J13+Логистика!J13+Прочее!J13</f>
+        <f>Sales!J13+Production!J13+Logistics!J13+Misc!J13</f>
         <v>117180</v>
       </c>
       <c r="K13" s="4">
-        <f>Продажи!K13+Производство!K13+Логистика!K13+Прочее!K13</f>
+        <f>Sales!K13+Production!K13+Logistics!K13+Misc!K13</f>
         <v>113627</v>
       </c>
       <c r="L13" s="4">
-        <f>Продажи!L13+Производство!L13+Логистика!L13+Прочее!L13</f>
+        <f>Sales!L13+Production!L13+Logistics!L13+Misc!L13</f>
         <v>115254</v>
       </c>
       <c r="M13" s="5">
-        <f>Продажи!M13+Производство!M13+Логистика!M13+Прочее!M13</f>
+        <f>Sales!M13+Production!M13+Logistics!M13+Misc!M13</f>
         <v>124461</v>
       </c>
       <c r="N13" s="6"/>
@@ -1930,56 +1930,56 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1">
       <c r="A14" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="11">
-        <f>Продажи!B14+Производство!B14+Логистика!B14+Прочее!B14</f>
+        <f>Sales!B14+Production!B14+Logistics!B14+Misc!B14</f>
         <v>21373</v>
       </c>
       <c r="C14" s="12">
-        <f>Продажи!C14+Производство!C14+Логистика!C14+Прочее!C14</f>
+        <f>Sales!C14+Production!C14+Logistics!C14+Misc!C14</f>
         <v>18311</v>
       </c>
       <c r="D14" s="12">
-        <f>Продажи!D14+Производство!D14+Логистика!D14+Прочее!D14</f>
+        <f>Sales!D14+Production!D14+Logistics!D14+Misc!D14</f>
         <v>19303</v>
       </c>
       <c r="E14" s="12">
-        <f>Продажи!E14+Производство!E14+Логистика!E14+Прочее!E14</f>
+        <f>Sales!E14+Production!E14+Logistics!E14+Misc!E14</f>
         <v>20622</v>
       </c>
       <c r="F14" s="12">
-        <f>Продажи!F14+Производство!F14+Логистика!F14+Прочее!F14</f>
+        <f>Sales!F14+Production!F14+Logistics!F14+Misc!F14</f>
         <v>20535</v>
       </c>
       <c r="G14" s="12">
-        <f>Продажи!G14+Производство!G14+Логистика!G14+Прочее!G14</f>
+        <f>Sales!G14+Production!G14+Logistics!G14+Misc!G14</f>
         <v>20817</v>
       </c>
       <c r="H14" s="12">
-        <f>Продажи!H14+Производство!H14+Логистика!H14+Прочее!H14</f>
+        <f>Sales!H14+Production!H14+Logistics!H14+Misc!H14</f>
         <v>19807</v>
       </c>
       <c r="I14" s="12">
-        <f>Продажи!I14+Производство!I14+Логистика!I14+Прочее!I14</f>
+        <f>Sales!I14+Production!I14+Logistics!I14+Misc!I14</f>
         <v>19531</v>
       </c>
       <c r="J14" s="12">
-        <f>Продажи!J14+Производство!J14+Логистика!J14+Прочее!J14</f>
+        <f>Sales!J14+Production!J14+Logistics!J14+Misc!J14</f>
         <v>20457</v>
       </c>
       <c r="K14" s="12">
-        <f>Продажи!K14+Производство!K14+Логистика!K14+Прочее!K14</f>
+        <f>Sales!K14+Production!K14+Logistics!K14+Misc!K14</f>
         <v>20186</v>
       </c>
       <c r="L14" s="12">
-        <f>Продажи!L14+Производство!L14+Логистика!L14+Прочее!L14</f>
+        <f>Sales!L14+Production!L14+Logistics!L14+Misc!L14</f>
         <v>21512</v>
       </c>
       <c r="M14" s="13">
-        <f>Продажи!M14+Производство!M14+Логистика!M14+Прочее!M14</f>
+        <f>Sales!M14+Production!M14+Logistics!M14+Misc!M14</f>
         <v>20964</v>
       </c>
       <c r="N14" s="6"/>
@@ -1988,7 +1988,7 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="28" customFormat="1" ht="15.75" thickBot="1">
       <c r="A15" s="20" t="s">
         <v>9</v>
       </c>
@@ -2046,7 +2046,7 @@
       <c r="Q15" s="26"/>
       <c r="R15" s="27"/>
     </row>
-    <row r="16" spans="1:18" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" s="28" customFormat="1" ht="15.75" thickBot="1">
       <c r="A16" s="20" t="s">
         <v>10</v>
       </c>
@@ -2104,7 +2104,7 @@
       <c r="Q16" s="26"/>
       <c r="R16" s="27"/>
     </row>
-    <row r="17" spans="1:18" s="58" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" s="58" customFormat="1" ht="15.75" thickBot="1">
       <c r="A17" s="52"/>
       <c r="B17" s="53"/>
       <c r="C17" s="54"/>
@@ -2124,8 +2124,8 @@
       <c r="Q17" s="56"/>
       <c r="R17" s="57"/>
     </row>
-    <row r="18" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="85" t="s">
+    <row r="18" spans="1:18" s="28" customFormat="1" ht="13">
+      <c r="A18" s="80" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="59"/>
@@ -2146,8 +2146,8 @@
       <c r="Q18" s="62"/>
       <c r="R18" s="63"/>
     </row>
-    <row r="19" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="86" t="s">
+    <row r="19" spans="1:18" s="28" customFormat="1" ht="13">
+      <c r="A19" s="81" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="64"/>
@@ -2168,8 +2168,8 @@
       <c r="Q19" s="67"/>
       <c r="R19" s="68"/>
     </row>
-    <row r="20" spans="1:18" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="87" t="s">
+    <row r="20" spans="1:18" s="28" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A20" s="82" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="69"/>
@@ -2214,60 +2214,60 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.625" customWidth="1"/>
-    <col min="2" max="13" width="8.625" customWidth="1"/>
-    <col min="14" max="18" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+    <col min="2" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="18" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="78" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1">
+      <c r="B1" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-    </row>
-    <row r="2" spans="1:18" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:18" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="74" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+    </row>
+    <row r="2" spans="1:18" s="28" customFormat="1" thickBot="1"/>
+    <row r="3" spans="1:18" s="28" customFormat="1">
+      <c r="B3" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="77"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="86"/>
       <c r="R3" s="33"/>
     </row>
-    <row r="4" spans="1:18" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="28" customFormat="1" thickBot="1">
       <c r="B4" s="34">
         <v>1</v>
       </c>
@@ -2310,7 +2310,7 @@
       <c r="Q4" s="37"/>
       <c r="R4" s="38"/>
     </row>
-    <row r="5" spans="1:18" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="28" customFormat="1">
       <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
@@ -2332,7 +2332,7 @@
       <c r="Q5" s="43"/>
       <c r="R5" s="44"/>
     </row>
-    <row r="6" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -2378,7 +2378,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -2400,7 +2400,7 @@
       <c r="Q7" s="18"/>
       <c r="R7" s="19"/>
     </row>
-    <row r="8" spans="1:18" s="28" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1">
       <c r="A8" s="20" t="s">
         <v>3</v>
       </c>
@@ -2422,7 +2422,7 @@
       <c r="Q8" s="26"/>
       <c r="R8" s="27"/>
     </row>
-    <row r="9" spans="1:18" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="28" customFormat="1">
       <c r="A9" s="39" t="s">
         <v>4</v>
       </c>
@@ -2444,7 +2444,7 @@
       <c r="Q9" s="50"/>
       <c r="R9" s="51"/>
     </row>
-    <row r="10" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -2466,7 +2466,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
@@ -2488,7 +2488,7 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -2534,7 +2534,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -2580,7 +2580,7 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1">
       <c r="A14" s="10" t="s">
         <v>6</v>
       </c>
@@ -2626,7 +2626,7 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" s="28" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1">
       <c r="A15" s="20" t="s">
         <v>9</v>
       </c>
@@ -2671,60 +2671,60 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.625" customWidth="1"/>
-    <col min="2" max="13" width="8.625" customWidth="1"/>
-    <col min="14" max="18" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+    <col min="2" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="18" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="78" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1">
+      <c r="B1" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-    </row>
-    <row r="2" spans="1:18" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:18" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="74" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+    </row>
+    <row r="2" spans="1:18" s="28" customFormat="1" thickBot="1"/>
+    <row r="3" spans="1:18" s="28" customFormat="1">
+      <c r="B3" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="77"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="86"/>
       <c r="R3" s="33"/>
     </row>
-    <row r="4" spans="1:18" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="28" customFormat="1" thickBot="1">
       <c r="B4" s="34">
         <v>1</v>
       </c>
@@ -2767,7 +2767,7 @@
       <c r="Q4" s="37"/>
       <c r="R4" s="38"/>
     </row>
-    <row r="5" spans="1:18" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="28" customFormat="1">
       <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
@@ -2789,7 +2789,7 @@
       <c r="Q5" s="43"/>
       <c r="R5" s="44"/>
     </row>
-    <row r="6" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -2811,7 +2811,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -2833,7 +2833,7 @@
       <c r="Q7" s="18"/>
       <c r="R7" s="19"/>
     </row>
-    <row r="8" spans="1:18" s="28" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1">
       <c r="A8" s="20" t="s">
         <v>3</v>
       </c>
@@ -2855,66 +2855,66 @@
       <c r="Q8" s="26"/>
       <c r="R8" s="27"/>
     </row>
-    <row r="9" spans="1:18" s="28" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1">
       <c r="A9" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="81"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="76"/>
       <c r="N9" s="48"/>
       <c r="O9" s="49"/>
       <c r="P9" s="49"/>
       <c r="Q9" s="50"/>
       <c r="R9" s="51"/>
     </row>
-    <row r="10" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="82">
+      <c r="B10" s="77">
         <v>250000</v>
       </c>
-      <c r="C10" s="83">
+      <c r="C10" s="78">
         <v>191250</v>
       </c>
-      <c r="D10" s="83">
+      <c r="D10" s="78">
         <v>150830.83333333334</v>
       </c>
-      <c r="E10" s="83">
+      <c r="E10" s="78">
         <v>185891.66666666669</v>
       </c>
-      <c r="F10" s="83">
+      <c r="F10" s="78">
         <v>100441.66666666667</v>
       </c>
-      <c r="G10" s="83">
+      <c r="G10" s="78">
         <v>139916.66666666669</v>
       </c>
-      <c r="H10" s="83">
+      <c r="H10" s="78">
         <v>187250</v>
       </c>
-      <c r="I10" s="83">
+      <c r="I10" s="78">
         <v>292139.16666666669</v>
       </c>
-      <c r="J10" s="83">
+      <c r="J10" s="78">
         <v>192239.16666666669</v>
       </c>
-      <c r="K10" s="83">
+      <c r="K10" s="78">
         <v>149120.83333333334</v>
       </c>
-      <c r="L10" s="83">
+      <c r="L10" s="78">
         <v>155583.33333333334</v>
       </c>
-      <c r="M10" s="84">
+      <c r="M10" s="79">
         <v>102791.66666666667</v>
       </c>
       <c r="N10" s="6"/>
@@ -2923,7 +2923,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
@@ -2945,7 +2945,7 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -2967,7 +2967,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -3013,7 +3013,7 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1">
       <c r="A14" s="10" t="s">
         <v>6</v>
       </c>
@@ -3059,7 +3059,7 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" s="28" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1">
       <c r="A15" s="20" t="s">
         <v>9</v>
       </c>
@@ -3104,60 +3104,60 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.625" customWidth="1"/>
-    <col min="2" max="13" width="8.625" customWidth="1"/>
-    <col min="14" max="18" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+    <col min="2" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="18" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="78" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1">
+      <c r="B1" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-    </row>
-    <row r="2" spans="1:18" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:18" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="74" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+    </row>
+    <row r="2" spans="1:18" s="28" customFormat="1" thickBot="1"/>
+    <row r="3" spans="1:18" s="28" customFormat="1">
+      <c r="B3" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="77"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="86"/>
       <c r="R3" s="33"/>
     </row>
-    <row r="4" spans="1:18" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="28" customFormat="1" thickBot="1">
       <c r="B4" s="34">
         <v>1</v>
       </c>
@@ -3200,7 +3200,7 @@
       <c r="Q4" s="37"/>
       <c r="R4" s="38"/>
     </row>
-    <row r="5" spans="1:18" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="28" customFormat="1">
       <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
@@ -3222,7 +3222,7 @@
       <c r="Q5" s="43"/>
       <c r="R5" s="44"/>
     </row>
-    <row r="6" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -3244,7 +3244,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -3266,7 +3266,7 @@
       <c r="Q7" s="18"/>
       <c r="R7" s="19"/>
     </row>
-    <row r="8" spans="1:18" s="28" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1">
       <c r="A8" s="20" t="s">
         <v>3</v>
       </c>
@@ -3288,7 +3288,7 @@
       <c r="Q8" s="26"/>
       <c r="R8" s="27"/>
     </row>
-    <row r="9" spans="1:18" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="28" customFormat="1">
       <c r="A9" s="39" t="s">
         <v>4</v>
       </c>
@@ -3310,7 +3310,7 @@
       <c r="Q9" s="50"/>
       <c r="R9" s="51"/>
     </row>
-    <row r="10" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -3332,7 +3332,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
@@ -3354,7 +3354,7 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -3376,7 +3376,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -3398,7 +3398,7 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1">
       <c r="A14" s="10" t="s">
         <v>6</v>
       </c>
@@ -3420,7 +3420,7 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" s="28" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1">
       <c r="A15" s="20" t="s">
         <v>9</v>
       </c>
@@ -3442,7 +3442,7 @@
       <c r="Q15" s="26"/>
       <c r="R15" s="27"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:5">
       <c r="E23" t="s">
         <v>15</v>
       </c>
@@ -3471,60 +3471,60 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.625" customWidth="1"/>
-    <col min="2" max="13" width="8.625" customWidth="1"/>
-    <col min="14" max="18" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+    <col min="2" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="18" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="78" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1">
+      <c r="B1" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-    </row>
-    <row r="2" spans="1:18" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:18" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="74" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+    </row>
+    <row r="2" spans="1:18" s="28" customFormat="1" thickBot="1"/>
+    <row r="3" spans="1:18" s="28" customFormat="1">
+      <c r="B3" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="77"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="86"/>
       <c r="R3" s="33"/>
     </row>
-    <row r="4" spans="1:18" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="28" customFormat="1" thickBot="1">
       <c r="B4" s="34">
         <v>1</v>
       </c>
@@ -3567,7 +3567,7 @@
       <c r="Q4" s="37"/>
       <c r="R4" s="38"/>
     </row>
-    <row r="5" spans="1:18" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="28" customFormat="1">
       <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
@@ -3589,7 +3589,7 @@
       <c r="Q5" s="43"/>
       <c r="R5" s="44"/>
     </row>
-    <row r="6" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -3611,7 +3611,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -3657,7 +3657,7 @@
       <c r="Q7" s="18"/>
       <c r="R7" s="19"/>
     </row>
-    <row r="8" spans="1:18" s="28" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1">
       <c r="A8" s="20" t="s">
         <v>3</v>
       </c>
@@ -3679,7 +3679,7 @@
       <c r="Q8" s="26"/>
       <c r="R8" s="27"/>
     </row>
-    <row r="9" spans="1:18" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="28" customFormat="1">
       <c r="A9" s="39" t="s">
         <v>4</v>
       </c>
@@ -3701,7 +3701,7 @@
       <c r="Q9" s="50"/>
       <c r="R9" s="51"/>
     </row>
-    <row r="10" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -3723,7 +3723,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
@@ -3745,7 +3745,7 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -3767,7 +3767,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" s="8" customFormat="1" ht="12">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -3813,7 +3813,7 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="8" customFormat="1" ht="12.75" thickBot="1">
       <c r="A14" s="10" t="s">
         <v>6</v>
       </c>
@@ -3859,7 +3859,7 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" s="28" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1">
       <c r="A15" s="20" t="s">
         <v>9</v>
       </c>

</xml_diff>